<commit_message>
adding full dataset 936
</commit_message>
<xml_diff>
--- a/2_data_processing/new_dict.xlsx
+++ b/2_data_processing/new_dict.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B217"/>
+  <dimension ref="A1:B221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +415,9 @@
           <t>population_total</t>
         </is>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -422,6 +425,9 @@
           <t>population_total_m</t>
         </is>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -429,6 +435,9 @@
           <t>population_total_f</t>
         </is>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -436,6 +445,9 @@
           <t>population_0_4_total</t>
         </is>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -443,6 +455,9 @@
           <t>population_0_4_total_m</t>
         </is>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -450,6 +465,9 @@
           <t>population_0_4_total_f</t>
         </is>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -457,6 +475,9 @@
           <t>population_5_9_total</t>
         </is>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -464,6 +485,9 @@
           <t>population_5_9_total_m</t>
         </is>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -471,6 +495,9 @@
           <t>population_5_9_total_f</t>
         </is>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -478,6 +505,9 @@
           <t>population_10_14_total</t>
         </is>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -485,6 +515,9 @@
           <t>population_10_14_total_m</t>
         </is>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -492,6 +525,9 @@
           <t>population_10_14_total_f</t>
         </is>
       </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -499,6 +535,9 @@
           <t>population_15_19_total</t>
         </is>
       </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -506,6 +545,9 @@
           <t>population_15_19_total_m</t>
         </is>
       </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -513,6 +555,9 @@
           <t>population_15_19_total_f</t>
         </is>
       </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -520,6 +565,9 @@
           <t>population_20_24_total</t>
         </is>
       </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -527,6 +575,9 @@
           <t>population_20_24_total_m</t>
         </is>
       </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -534,6 +585,9 @@
           <t>population_20_24_total_f</t>
         </is>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -541,6 +595,9 @@
           <t>population_25_29_total</t>
         </is>
       </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -548,6 +605,9 @@
           <t>population_25_29_total_m</t>
         </is>
       </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -555,6 +615,9 @@
           <t>population_25_29_total_f</t>
         </is>
       </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -562,6 +625,9 @@
           <t>population_30_34_total</t>
         </is>
       </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -569,6 +635,9 @@
           <t>population_30_34_total_m</t>
         </is>
       </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -576,6 +645,9 @@
           <t>population_30_34_total_f</t>
         </is>
       </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -583,6 +655,9 @@
           <t>population_35_39_total</t>
         </is>
       </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -590,6 +665,9 @@
           <t>population_35_39_total_m</t>
         </is>
       </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -597,6 +675,9 @@
           <t>population_35_39_total_f</t>
         </is>
       </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -604,6 +685,9 @@
           <t>population_40_44_total</t>
         </is>
       </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -611,6 +695,9 @@
           <t>population_40_44_total_m</t>
         </is>
       </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -618,6 +705,9 @@
           <t>population_40_44_total_f</t>
         </is>
       </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -625,6 +715,9 @@
           <t>population_45_49_total</t>
         </is>
       </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -632,6 +725,9 @@
           <t>population_45_49_total_m</t>
         </is>
       </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -639,6 +735,9 @@
           <t>population_45_49_total_f</t>
         </is>
       </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -646,6 +745,9 @@
           <t>population_50_54_total</t>
         </is>
       </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -653,6 +755,9 @@
           <t>population_50_54_total_m</t>
         </is>
       </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -660,6 +765,9 @@
           <t>population_50_54_total_f</t>
         </is>
       </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -667,6 +775,9 @@
           <t>population_55_59_total</t>
         </is>
       </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -674,6 +785,9 @@
           <t>population_55_59_total_m</t>
         </is>
       </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -681,6 +795,9 @@
           <t>population_55_59_total_f</t>
         </is>
       </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -688,6 +805,9 @@
           <t>population_60_64_total</t>
         </is>
       </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -695,6 +815,9 @@
           <t>population_60_64_total_m</t>
         </is>
       </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -702,6 +825,9 @@
           <t>population_60_64_total_f</t>
         </is>
       </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -709,6 +835,9 @@
           <t>population_65_69_total</t>
         </is>
       </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -716,6 +845,9 @@
           <t>population_65_69_total_m</t>
         </is>
       </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -723,6 +855,9 @@
           <t>population_65_69_total_f</t>
         </is>
       </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -730,6 +865,9 @@
           <t>population_70_74_total</t>
         </is>
       </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -737,6 +875,9 @@
           <t>population_70_74_total_m</t>
         </is>
       </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -744,6 +885,9 @@
           <t>population_70_74_total_f</t>
         </is>
       </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -751,6 +895,9 @@
           <t>population_75_79_total</t>
         </is>
       </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -758,6 +905,9 @@
           <t>population_75_79_total_m</t>
         </is>
       </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -765,6 +915,9 @@
           <t>population_75_79_total_f</t>
         </is>
       </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -772,6 +925,9 @@
           <t>population_80_84_total</t>
         </is>
       </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -779,6 +935,9 @@
           <t>population_80_84_total_m</t>
         </is>
       </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -786,6 +945,9 @@
           <t>population_80_84_total_f</t>
         </is>
       </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -803,6 +965,9 @@
           <t>population_density</t>
         </is>
       </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -830,6 +995,9 @@
           <t>population_per_pharmacy</t>
         </is>
       </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -857,6 +1025,9 @@
           <t>installations_bathroom</t>
         </is>
       </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -884,6 +1055,9 @@
           <t>appartment_area_per_person</t>
         </is>
       </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -891,6 +1065,9 @@
           <t>appartments_per_1000_persons</t>
         </is>
       </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -908,6 +1085,9 @@
           <t>persons_per_room</t>
         </is>
       </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -965,6 +1145,9 @@
           <t>unemployed_total</t>
         </is>
       </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -972,6 +1155,9 @@
           <t>unemployed_f</t>
         </is>
       </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -979,6 +1165,9 @@
           <t>unemployed_m</t>
         </is>
       </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -986,6 +1175,9 @@
           <t>unemployed_up_to_25</t>
         </is>
       </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -993,6 +1185,9 @@
           <t>unemployed_over_50</t>
         </is>
       </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1000,6 +1195,9 @@
           <t>unemployed_long_term</t>
         </is>
       </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1007,6 +1205,9 @@
           <t>unemployment_rate</t>
         </is>
       </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1014,6 +1215,9 @@
           <t>unemployment_rate_m</t>
         </is>
       </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1021,6 +1225,9 @@
           <t>unemployment_rate_f</t>
         </is>
       </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1048,6 +1255,9 @@
           <t>revenues_per_capita</t>
         </is>
       </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1075,6 +1285,9 @@
           <t>expenditures_per_capita</t>
         </is>
       </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1102,6 +1315,9 @@
           <t>net_scholarization</t>
         </is>
       </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1139,6 +1355,9 @@
           <t>persons_running_business</t>
         </is>
       </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1176,6 +1395,9 @@
           <t>Austrian</t>
         </is>
       </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1183,6 +1405,9 @@
           <t>teryt_gmina</t>
         </is>
       </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1190,6 +1415,9 @@
           <t>gmina</t>
         </is>
       </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1197,6 +1425,9 @@
           <t>powiat</t>
         </is>
       </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1204,6 +1435,9 @@
           <t>województwo</t>
         </is>
       </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1231,6 +1465,9 @@
           <t>glosy_niewazne_1</t>
         </is>
       </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1238,6 +1475,9 @@
           <t>glosy_niewazne_2</t>
         </is>
       </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1245,6 +1485,9 @@
           <t>glosy_niewazne_3</t>
         </is>
       </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1252,6 +1495,9 @@
           <t>glosy_wazne</t>
         </is>
       </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1289,6 +1535,9 @@
           <t>glosy_PIS</t>
         </is>
       </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1306,6 +1555,9 @@
           <t>pop_t_0_4_perc</t>
         </is>
       </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -1313,6 +1565,9 @@
           <t>pop_m_0_4_perc</t>
         </is>
       </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -1320,6 +1575,9 @@
           <t>pop_f_0_4_perc</t>
         </is>
       </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -1327,6 +1585,9 @@
           <t>pop_t_5_9_perc</t>
         </is>
       </c>
+      <c r="B123">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -1334,6 +1595,9 @@
           <t>pop_m_5_9_perc</t>
         </is>
       </c>
+      <c r="B124">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -1341,6 +1605,9 @@
           <t>pop_f_5_9_perc</t>
         </is>
       </c>
+      <c r="B125">
+        <v>1</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -1348,6 +1615,9 @@
           <t>pop_t_10_14_perc</t>
         </is>
       </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -1355,6 +1625,9 @@
           <t>pop_m_10_14_perc</t>
         </is>
       </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -1362,6 +1635,9 @@
           <t>pop_f_10_14_perc</t>
         </is>
       </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -1369,6 +1645,9 @@
           <t>pop_t_15_19_perc</t>
         </is>
       </c>
+      <c r="B129">
+        <v>1</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -1376,6 +1655,9 @@
           <t>pop_m_15_19_perc</t>
         </is>
       </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -1383,6 +1665,9 @@
           <t>pop_f_15_19_perc</t>
         </is>
       </c>
+      <c r="B131">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -1390,6 +1675,9 @@
           <t>pop_t_20_24_perc</t>
         </is>
       </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -1397,6 +1685,9 @@
           <t>pop_m_20_24_perc</t>
         </is>
       </c>
+      <c r="B133">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -1404,6 +1695,9 @@
           <t>pop_f_20_24_perc</t>
         </is>
       </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -1411,6 +1705,9 @@
           <t>pop_t_25_29_perc</t>
         </is>
       </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -1418,6 +1715,9 @@
           <t>pop_m_25_29_perc</t>
         </is>
       </c>
+      <c r="B136">
+        <v>1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -1425,6 +1725,9 @@
           <t>pop_f_25_29_perc</t>
         </is>
       </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -1432,6 +1735,9 @@
           <t>pop_t_30_34_perc</t>
         </is>
       </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -1439,6 +1745,9 @@
           <t>pop_m_30_34_perc</t>
         </is>
       </c>
+      <c r="B139">
+        <v>1</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -1446,6 +1755,9 @@
           <t>pop_f_30_34_perc</t>
         </is>
       </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -1453,6 +1765,9 @@
           <t>pop_t_35_39_perc</t>
         </is>
       </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -1460,6 +1775,9 @@
           <t>pop_m_35_39_perc</t>
         </is>
       </c>
+      <c r="B142">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -1467,6 +1785,9 @@
           <t>pop_f_35_39_perc</t>
         </is>
       </c>
+      <c r="B143">
+        <v>1</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -1474,6 +1795,9 @@
           <t>pop_t_40_44_perc</t>
         </is>
       </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -1481,6 +1805,9 @@
           <t>pop_m_40_44_perc</t>
         </is>
       </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -1488,6 +1815,9 @@
           <t>pop_f_40_44_perc</t>
         </is>
       </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -1495,6 +1825,9 @@
           <t>pop_t_45_49_perc</t>
         </is>
       </c>
+      <c r="B147">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -1502,6 +1835,9 @@
           <t>pop_m_45_49_perc</t>
         </is>
       </c>
+      <c r="B148">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -1509,6 +1845,9 @@
           <t>pop_f_45_49_perc</t>
         </is>
       </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -1516,6 +1855,9 @@
           <t>pop_t_50_54_perc</t>
         </is>
       </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -1523,6 +1865,9 @@
           <t>pop_m_50_54_perc</t>
         </is>
       </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -1530,6 +1875,9 @@
           <t>pop_f_50_54_perc</t>
         </is>
       </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -1537,6 +1885,9 @@
           <t>pop_t_55_59_perc</t>
         </is>
       </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -1544,6 +1895,9 @@
           <t>pop_m_55_59_perc</t>
         </is>
       </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -1551,6 +1905,9 @@
           <t>pop_f_55_59_perc</t>
         </is>
       </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -1558,6 +1915,9 @@
           <t>pop_t_60_64_perc</t>
         </is>
       </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -1565,6 +1925,9 @@
           <t>pop_m_60_64_perc</t>
         </is>
       </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -1572,6 +1935,9 @@
           <t>pop_f_60_64_perc</t>
         </is>
       </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -1579,6 +1945,9 @@
           <t>pop_t_65_69_perc</t>
         </is>
       </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -1586,6 +1955,9 @@
           <t>pop_m_65_69_perc</t>
         </is>
       </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -1593,6 +1965,9 @@
           <t>pop_f_65_69_perc</t>
         </is>
       </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -1600,6 +1975,9 @@
           <t>pop_t_70_74_perc</t>
         </is>
       </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -1607,6 +1985,9 @@
           <t>pop_m_70_74_perc</t>
         </is>
       </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -1614,6 +1995,9 @@
           <t>pop_f_70_74_perc</t>
         </is>
       </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -1621,6 +2005,9 @@
           <t>pop_t_75_79_perc</t>
         </is>
       </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -1628,6 +2015,9 @@
           <t>pop_m_75_79_perc</t>
         </is>
       </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -1635,6 +2025,9 @@
           <t>pop_f_75_79_perc</t>
         </is>
       </c>
+      <c r="B167">
+        <v>1</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -1642,6 +2035,9 @@
           <t>pop_t_80_84_perc</t>
         </is>
       </c>
+      <c r="B168">
+        <v>1</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -1649,6 +2045,9 @@
           <t>pop_m_80_84_perc</t>
         </is>
       </c>
+      <c r="B169">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -1656,6 +2055,9 @@
           <t>pop_f_80_84_perc</t>
         </is>
       </c>
+      <c r="B170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -1673,6 +2075,9 @@
           <t>pop_m_0_19_perc</t>
         </is>
       </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -1680,6 +2085,9 @@
           <t>pop_f_0_19_perc</t>
         </is>
       </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -1697,6 +2105,9 @@
           <t>pop_m_40_49_perc</t>
         </is>
       </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -1704,6 +2115,9 @@
           <t>pop_f_40_49_perc</t>
         </is>
       </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -1721,6 +2135,9 @@
           <t>pop_m_20_29_perc</t>
         </is>
       </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -1728,6 +2145,9 @@
           <t>pop_f_20_29_perc</t>
         </is>
       </c>
+      <c r="B179">
+        <v>1</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -1735,6 +2155,9 @@
           <t>pop_t_30_39_perc</t>
         </is>
       </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -1742,6 +2165,9 @@
           <t>pop_m_30_39_perc</t>
         </is>
       </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -1749,6 +2175,9 @@
           <t>pop_f_30_39_perc</t>
         </is>
       </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -1766,6 +2195,9 @@
           <t>pop_m_50_59_perc</t>
         </is>
       </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -1773,6 +2205,9 @@
           <t>pop_f_50_59_perc</t>
         </is>
       </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -1790,6 +2225,9 @@
           <t>pop_m_60_84_perc</t>
         </is>
       </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -1797,6 +2235,9 @@
           <t>pop_f_60_84_perc</t>
         </is>
       </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -1804,6 +2245,9 @@
           <t>pop_m_all_perc</t>
         </is>
       </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -1821,6 +2265,9 @@
           <t>id</t>
         </is>
       </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -1828,6 +2275,9 @@
           <t>name</t>
         </is>
       </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -1835,6 +2285,9 @@
           <t>year</t>
         </is>
       </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -1842,6 +2295,9 @@
           <t>podatek_rolny</t>
         </is>
       </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -1899,6 +2355,9 @@
           <t>county_name</t>
         </is>
       </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -1986,6 +2445,9 @@
           <t>education_share_primary</t>
         </is>
       </c>
+      <c r="B209">
+        <v>1</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -2020,7 +2482,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>type_agr</t>
+          <t>last_n</t>
         </is>
       </c>
       <c r="B213">
@@ -2030,7 +2492,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>type_0_20k</t>
+          <t>type_1</t>
         </is>
       </c>
       <c r="B214">
@@ -2040,7 +2502,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>type_50_100k</t>
+          <t>type_2</t>
         </is>
       </c>
       <c r="B215">
@@ -2050,7 +2512,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>type_500k+</t>
+          <t>type_20_50k</t>
         </is>
       </c>
       <c r="B216">
@@ -2060,10 +2522,50 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
+          <t>type_agr</t>
+        </is>
+      </c>
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>type_0_20k</t>
+        </is>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>type_50_100k</t>
+        </is>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>type_500k+</t>
+        </is>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
           <t>type_100_500k</t>
         </is>
       </c>
-      <c r="B217">
+      <c r="B221">
         <v>1</v>
       </c>
     </row>

</xml_diff>